<commit_message>
Mother and child wing plans
Need to make mother and child file
Make updated life history complete data file and run R again
</commit_message>
<xml_diff>
--- a/Wing results/Landmark descriptions.xlsx
+++ b/Wing results/Landmark descriptions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Landmark #</t>
   </si>
@@ -42,6 +42,36 @@
   </si>
   <si>
     <t>III</t>
+  </si>
+  <si>
+    <t>http://ihi.eprints.org/1274/1/Gillies_&amp;_Coetzee_1984_Supplement_to_African_anophelines_1.pdf</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Comstock%E2%80%93Needham_system</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 2.1</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 2.2</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 3</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 4.1</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 4.2</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 5.1</t>
+  </si>
+  <si>
+    <t>Distal end of Rs 5.2</t>
+  </si>
+  <si>
+    <t>Proximal end of Rs 5.1 and 5.2</t>
   </si>
 </sst>
 </file>
@@ -95,6 +125,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>538266</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40F4A813-7E0B-4DBF-A3A7-CE4496E4F2AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5610225" y="762000"/>
+          <a:ext cx="8463066" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,15 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -447,6 +527,9 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -455,6 +538,9 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -463,6 +549,9 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -471,6 +560,9 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -479,6 +571,9 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -487,6 +582,9 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -495,6 +593,9 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -503,6 +604,9 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -528,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
@@ -536,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>16</v>
       </c>
@@ -544,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>17</v>
       </c>
@@ -552,16 +656,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>